<commit_message>
changed period for downscaled PDFs
climatological period: 1993-2019
future period: 2060-2080
</commit_message>
<xml_diff>
--- a/data/Downscaleddata/pdfs/bottom o2_thresholds.xlsx
+++ b/data/Downscaleddata/pdfs/bottom o2_thresholds.xlsx
@@ -496,10 +496,10 @@
         <v>1.100385049623747</v>
       </c>
       <c r="D2" t="n">
-        <v>3.542583507443938</v>
+        <v>3.479888236813032</v>
       </c>
       <c r="E2" t="n">
-        <v>1.045389290513603</v>
+        <v>0.8548164319983614</v>
       </c>
       <c r="F2" t="n">
         <v>3.524883908303043</v>
@@ -508,10 +508,10 @@
         <v>0.6629871557899286</v>
       </c>
       <c r="H2" t="n">
-        <v>3.347340434915449</v>
+        <v>3.341511580334618</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9275548951266984</v>
+        <v>0.7582507812126756</v>
       </c>
       <c r="J2" t="n">
         <v>3.323323020455365</v>

</xml_diff>